<commit_message>
ajustado sem os arquivos credenciais
</commit_message>
<xml_diff>
--- a/Suporte-ThermoSafeHidraulico-v01.xlsx
+++ b/Suporte-ThermoSafeHidraulico-v01.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="261">
   <si>
     <t>A) Criar o projeto e preparar o Firestore (cloud)</t>
   </si>
@@ -3741,6 +3741,12 @@
   </si>
   <si>
     <t>pip install pandas openpyxl --upgrade</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> git rm -r --cached .github Sigiloso</t>
+  </si>
+  <si>
+    <t>não github de diretorio sigiloso</t>
   </si>
 </sst>
 </file>
@@ -5576,10 +5582,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:C97"/>
+  <dimension ref="B5:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5807,9 +5813,17 @@
     <row r="96" spans="2:2">
       <c r="B96" s="2"/>
     </row>
-    <row r="97" spans="2:2">
+    <row r="97" spans="2:3">
       <c r="B97" s="26" t="s">
         <v>256</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3">
+      <c r="B101" t="s">
+        <v>259</v>
+      </c>
+      <c r="C101" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>